<commit_message>
ajout de form.js dans le plan de test
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Projets Pro\DevWeb\Projet 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5DFA2A-5852-4C79-A5B5-A42D0887A9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA12310-0765-45A6-9F4D-CCF8050FF152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4995" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{395A17A5-375E-44D6-9666-28EF1ED33A10}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="406">
   <si>
     <t>Test unitaire</t>
   </si>
@@ -1282,6 +1282,71 @@
     <t>Appeler la fonction sur un élément cliquable du DOM (un button par exemple) :
      avec qty &lt;= 0 =&gt; l'élément devient inaccessible
      puis avec qty &gt; 0 =&gt; l'élément devient de nouveau accessible</t>
+  </si>
+  <si>
+    <t>listenFormInputsChanges ()</t>
+  </si>
+  <si>
+    <t>deleteError (input)</t>
+  </si>
+  <si>
+    <t>displayError (input)</t>
+  </si>
+  <si>
+    <t>toggleError (input, test)</t>
+  </si>
+  <si>
+    <t>form.js</t>
+  </si>
+  <si>
+    <t>25-33</t>
+  </si>
+  <si>
+    <t>42-47</t>
+  </si>
+  <si>
+    <t>49-59</t>
+  </si>
+  <si>
+    <t>input : un élément du DOM (de préférence un input)
+test : un booléen</t>
+  </si>
+  <si>
+    <t>met en place des listeners sur tous les inputs ayant les classes "form" et "input"
+Pour chacun de ces inputs, le listener surveille les changements et affiche une erreur si l'input est mal rempli</t>
+  </si>
+  <si>
+    <t>enlève le message d'erreur</t>
+  </si>
+  <si>
+    <t>affiche un message d'erreur</t>
+  </si>
+  <si>
+    <t>bascule entre l'affichage et la suppression du message d'erreur en fonction de la valeur du test</t>
+  </si>
+  <si>
+    <t>Entrer une valeur incorrecte dans chaque input concerné et vérifier qu'un message d'erreur est bien affiché (faire un test par valeur incorrecte).
+Puis saisir une valeur correcte et vérifier que le message d'erreur disparait bien</t>
+  </si>
+  <si>
+    <t>Appeler cette fonction sur un input qui a un message d'erreur et vérifier que le message disparaît</t>
+  </si>
+  <si>
+    <t>Appeler cette fonction sur un input qui n'a pas de message d'erreur et vérifier que le message apparaît</t>
+  </si>
+  <si>
+    <t>Appeler cette fonction sur un input avec des valeurs de test successivement à false puis true puis false
+=&gt; le message d'erreur disparaît puis apparaît puis disparaît</t>
+  </si>
+  <si>
+    <t>Aucun message ou un mauvais message d'erreur apparaît.
+Un message d'erreur apparait même si la valeur de l'input est correcte.</t>
+  </si>
+  <si>
+    <t>Aucun message ou un mauvais message d'erreur apparaît.</t>
+  </si>
+  <si>
+    <t>Le message d'erreur n'est pas supprimé.</t>
   </si>
 </sst>
 </file>
@@ -1747,11 +1812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526789AE-0D5F-4142-9833-DA4048E4C93D}">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="53.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3648,6 +3713,98 @@
         <v>259</v>
       </c>
     </row>
+    <row r="83" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>